<commit_message>
Nullable<T> works with both Enum and Complex
</commit_message>
<xml_diff>
--- a/Source/Samples/Registration.Sample/Registration.Samples.xlsx
+++ b/Source/Samples/Registration.Sample/Registration.Samples.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Tests for Complex</t>
   </si>
@@ -54,6 +54,18 @@
   </si>
   <si>
     <t>Expected values</t>
+  </si>
+  <si>
+    <t>empty cells in input array are considered as 0</t>
+  </si>
+  <si>
+    <t>a single input cell with #NA! is considered as null</t>
+  </si>
+  <si>
+    <t>but an input array full of #NA! should cause a conversion error</t>
+  </si>
+  <si>
+    <t>Inputs</t>
   </si>
 </sst>
 </file>
@@ -414,42 +426,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="e">
-        <f>AND(A4:A12)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" t="b">
+        <f>AND(A4:A15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <f>SUMSQ(B4:C4)&lt;0.00000000000001</f>
         <v>1</v>
       </c>
       <c r="B4">
-        <f>D4-G4</f>
+        <f t="shared" ref="B4:C9" si="0">D4-G4</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f>E4-H4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4">
@@ -466,17 +481,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <f>SUMSQ(B5:C5)&lt;0.00000000000001</f>
         <v>1</v>
       </c>
       <c r="B5">
-        <f>D5-G5</f>
+        <f t="shared" ref="B5:C8" si="1">D5-G5</f>
         <v>0</v>
       </c>
       <c r="C5">
-        <f>E5-H5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D5">
@@ -492,155 +507,267 @@
       <c r="H5">
         <v>222</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="e">
+      <c r="M5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="b">
         <f>SUMSQ(B6:C6)&lt;0.00000000000001</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B6" t="e">
-        <f>D6-G6</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C6" t="e">
-        <f>E6-H6</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D6" t="e">
-        <f t="array" ref="D6:E6">_xll.dnaNullableComplex(G6:H6)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E6" t="e">
-        <v>#NUM!</v>
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="array" ref="D6:E6">_xll.dnaNullableComplex(J6:K6)</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="b">
+        <f>SUMSQ(B7:C7)&lt;0.00000000000001</f>
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ref="B7" si="2">D7-G7</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7" si="3">E7-H7</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="array" ref="D7:E7">_xll.dnaNullableComplex(J7)</f>
+        <v>111</v>
+      </c>
+      <c r="E7">
+        <v>222</v>
+      </c>
+      <c r="G7">
+        <v>111</v>
+      </c>
+      <c r="H7">
+        <v>222</v>
+      </c>
+      <c r="J7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="b">
+        <f>SUMSQ(B8:C8)&lt;0.00000000000001</f>
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ref="B8" si="4">D8-G8</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8" si="5">E8-H8</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="array" ref="D8:E8">ERROR.TYPE(_xll.dnaNullableComplex(J8:K8))</f>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <f>ERROR.TYPE(#NUM!)</f>
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="J8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="b">
         <f>SUMSQ(B9:C9)&lt;0.00000000000001</f>
         <v>1</v>
       </c>
       <c r="B9">
-        <f>D9-G9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C9">
-        <f>E9-H9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="array" ref="D9:E9">_xll.dnaNullableEnum()</f>
-        <v>0</v>
+        <f t="array" ref="D9:E9">_xll.dnaNullableComplex(G9:H9)</f>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
       </c>
       <c r="M9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="b">
+        <f>SUMSQ(B12:C12)&lt;0.00000000000001</f>
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:C15" si="6">D12-G12</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="array" ref="D12:E12">_xll.dnaNullableEnum()</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="e">
-        <f>SUMSQ(B10:C10)&lt;0.00000000000001</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B10" t="e">
-        <f>D10-G10</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C10" t="e">
-        <f>E10-H10</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D10" t="e">
-        <f t="array" ref="D10:E10">_xll.dnaNullableEnum(J10,K10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="M10" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="b">
+        <f>SUMSQ(B13:C13)&lt;0.00000000000001</f>
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="array" ref="D13:E13">_xll.dnaNullableEnum(J13,K13)</f>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="e">
-        <f>SUMSQ(B11:C11)&lt;0.00000000000001</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B11" t="e">
-        <f>D11-G11</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C11" t="e">
-        <f>E11-H11</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D11" t="e">
-        <f t="array" ref="D11:E11">_xll.dnaNullableEnum(J11,K11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E11" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="J11" t="e">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="b">
+        <f>SUMSQ(B14:C14)&lt;0.00000000000001</f>
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="array" ref="D14:E14">_xll.dnaNullableEnum(J14,K14)</f>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="K11" t="e">
+      <c r="K14" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="e">
-        <f>SUMSQ(B12:C12)&lt;0.00000000000001</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="B12" t="e">
-        <f>D12-G12</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C12" t="e">
-        <f>E12-H12</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D12" t="e">
-        <f t="array" ref="D12:E12">_xll.dnaNullableEnum(J12,K12)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E12" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="G12">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="b">
+        <f>SUMSQ(B15:C15)&lt;0.00000000000001</f>
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="array" ref="D15:E15">_xll.dnaNullableEnum(J15,K15)</f>
         <v>-1</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>-1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
         <v>3</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K15" t="s">
         <v>4</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M15" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MarshalByRef works for return types
</commit_message>
<xml_diff>
--- a/Source/Samples/Registration.Sample/Registration.Samples.xlsx
+++ b/Source/Samples/Registration.Sample/Registration.Samples.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Tests for Complex</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Inputs</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
   </si>
 </sst>
 </file>
@@ -426,15 +435,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -443,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,17 +466,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
-        <f>SUMSQ(B4:C4)&lt;0.00000000000001</f>
+        <f t="shared" ref="A4:A9" si="0">SUMSQ(B4:C4)&lt;0.00000000000001</f>
         <v>1</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:C9" si="0">D4-G4</f>
+        <f t="shared" ref="B4:C9" si="1">D4-G4</f>
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D4">
@@ -481,17 +493,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
-        <f>SUMSQ(B5:C5)&lt;0.00000000000001</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:C8" si="1">D5-G5</f>
+        <f t="shared" ref="B5:C6" si="2">D5-G5</f>
         <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D5">
@@ -511,17 +523,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
-        <f>SUMSQ(B6:C6)&lt;0.00000000000001</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D6">
@@ -541,17 +553,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
-        <f>SUMSQ(B7:C7)&lt;0.00000000000001</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7" si="2">D7-G7</f>
+        <f t="shared" ref="B7" si="3">D7-G7</f>
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7" si="3">E7-H7</f>
+        <f t="shared" ref="C7" si="4">E7-H7</f>
         <v>0</v>
       </c>
       <c r="D7">
@@ -575,17 +587,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="b">
-        <f>SUMSQ(B8:C8)&lt;0.00000000000001</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8" si="4">D8-G8</f>
+        <f t="shared" ref="B8" si="5">D8-G8</f>
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8" si="5">E8-H8</f>
+        <f t="shared" ref="C8" si="6">E8-H8</f>
         <v>0</v>
       </c>
       <c r="D8">
@@ -614,17 +626,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="b">
-        <f>SUMSQ(B9:C9)&lt;0.00000000000001</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D9">
@@ -644,7 +656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -655,17 +667,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="b">
         <f>SUMSQ(B12:C12)&lt;0.00000000000001</f>
         <v>1</v>
       </c>
       <c r="B12">
-        <f t="shared" ref="B12:C15" si="6">D12-G12</f>
+        <f t="shared" ref="B12:C15" si="7">D12-G12</f>
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D12">
@@ -679,17 +691,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="b">
         <f>SUMSQ(B13:C13)&lt;0.00000000000001</f>
         <v>1</v>
       </c>
       <c r="B13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D13">
@@ -703,17 +715,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="b">
         <f>SUMSQ(B14:C14)&lt;0.00000000000001</f>
         <v>1</v>
       </c>
       <c r="B14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D14">
@@ -735,17 +747,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="b">
         <f>SUMSQ(B15:C15)&lt;0.00000000000001</f>
         <v>1</v>
       </c>
       <c r="B15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D15">
@@ -769,6 +781,40 @@
       </c>
       <c r="M15" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="e">
+        <f t="array" ref="A17:A19">_xll.dnaFactory(C17:C19,D17:D19)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <v>Exception has been thrown by the target of an invocation.</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Marshal-by-ref now works for both single objects and IEnumerable's
</commit_message>
<xml_diff>
--- a/Source/Samples/Registration.Sample/Registration.Samples.xlsx
+++ b/Source/Samples/Registration.Sample/Registration.Samples.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Tests for Complex</t>
   </si>
@@ -74,7 +74,13 @@
     <t>Two</t>
   </si>
   <si>
-    <t>Three</t>
+    <t>Marshal by reference</t>
+  </si>
+  <si>
+    <t>One call returning IEnumerable&lt;T&gt;</t>
+  </si>
+  <si>
+    <t>Multiple calls returning T</t>
   </si>
 </sst>
 </file>
@@ -435,15 +441,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -451,7 +458,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="b">
-        <f>AND(A4:A15)</f>
+        <f>AND(A4:A26)</f>
         <v>1</v>
       </c>
     </row>
@@ -783,38 +790,175 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="e">
-        <f t="array" ref="A17:A19">_xll.dnaFactory(C17:C19,D17:D19)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D18" t="str">
+        <f t="array" ref="D18:D20">_xll.dnaFactoryMultiple(E18:E20,F18:F20)</f>
+        <v>SampleClass1@3359</v>
+      </c>
+      <c r="E18" t="s">
         <v>14</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
-        <v>Exception has been thrown by the target of an invocation.</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="str">
+        <f>_xll.dnaFactorySingle(E18,F18)</f>
+        <v>SampleClass1@3367</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D19" t="str">
+        <v>SampleClass2@3360</v>
+      </c>
+      <c r="E19" t="s">
         <v>15</v>
       </c>
-      <c r="D18">
+      <c r="F19">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19">
+      <c r="G19" t="str">
+        <f>_xll.dnaFactorySingle(E19,F19)</f>
+        <v>SampleClass2@3357</v>
+      </c>
+      <c r="J19" t="str">
+        <f>_xll.dnaFactoryCompound(G19,G18)</f>
+        <v>Compound@3368</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D20" t="str">
+        <v>SampleClass1@3361</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20">
         <v>3</v>
+      </c>
+      <c r="G20" t="str">
+        <f>_xll.dnaFactorySingle(E20,F20)</f>
+        <v>SampleClass1@3358</v>
+      </c>
+      <c r="J20" t="str">
+        <f>_xll.dnaFactoryCompound(J19,G20)</f>
+        <v>Compound@3369</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="b">
+        <f>SUMSQ(B21:C21)&lt;0.00000000000001</f>
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ref="B21:C21" si="8">D21-G21</f>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f>G21-J21</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f>_xll.dnaMarshalByRef(D18:D20)</f>
+        <v>8</v>
+      </c>
+      <c r="G21">
+        <f>_xll.dnaMarshalByRef(G18:G20)</f>
+        <v>8</v>
+      </c>
+      <c r="J21">
+        <f>_xll.dnaMarshalByRef(J20)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D23" t="str">
+        <f t="array" ref="D23:D25">_xll.dnaFactoryMultiple(E23:E25,F23:F25)</f>
+        <v>SampleClass2@3370</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23" t="str">
+        <f>_xll.dnaFactorySingle(E23,F23)</f>
+        <v>SampleClass2@3362</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D24" t="str">
+        <v>SampleClass1@3371</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+      <c r="G24" t="str">
+        <f>_xll.dnaFactorySingle(E24,F24)</f>
+        <v>SampleClass1@3363</v>
+      </c>
+      <c r="J24" t="str">
+        <f>_xll.dnaFactoryCompound(G24,G23)</f>
+        <v>Compound@3364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D25" t="str">
+        <v>SampleClass2@3372</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25" t="str">
+        <f>_xll.dnaFactorySingle(E25,F25)</f>
+        <v>SampleClass2@3365</v>
+      </c>
+      <c r="J25" t="str">
+        <f>_xll.dnaFactoryCompound(J24,G25)</f>
+        <v>Compound@3366</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="b">
+        <f>SUMSQ(B26:C26)&lt;0.00000000000001</f>
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ref="B26" si="9">D26-G26</f>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f>G26-J26</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f>_xll.dnaMarshalByRef(D23:D25)</f>
+        <v>57</v>
+      </c>
+      <c r="G26">
+        <f>_xll.dnaMarshalByRef(G23:G25)</f>
+        <v>57</v>
+      </c>
+      <c r="J26">
+        <f>_xll.dnaMarshalByRef(J25)</f>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change to LambdaExpression registration available in Excel-DNA 1.2
</commit_message>
<xml_diff>
--- a/Source/Samples/Registration.Sample/Registration.Samples.xlsx
+++ b/Source/Samples/Registration.Sample/Registration.Samples.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23604"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amass\Documents\Visual Studio 2015\Projects\Registration\Source\Samples\Registration.Sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Excel-DNA\Registration\Source\Samples\Registration.Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2985513-21B9-43B4-B3BA-ED99928EBFD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8940"/>
+    <workbookView xWindow="5700" yWindow="3345" windowWidth="22080" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -84,7 +93,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -438,14 +447,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>